<commit_message>
Pappel 2 Android, iOS & RN Loc done with tests
</commit_message>
<xml_diff>
--- a/test/fixtures/XLSX2.xlsx
+++ b/test/fixtures/XLSX2.xlsx
@@ -34,7 +34,7 @@
     <t>hello you</t>
   </si>
   <si>
-    <t>Bonjout toi !</t>
+    <t>Bonjour toi !</t>
   </si>
   <si>
     <t>Hello you!</t>
@@ -130,6 +130,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>